<commit_message>
Updated the necropsy raw files with the correct process IDs.
</commit_message>
<xml_diff>
--- a/raw/necropsy/20250714_r2_GR_USDA-LNs_RT-QuIC.xlsx
+++ b/raw/necropsy/20250714_r2_GR_USDA-LNs_RT-QuIC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MNPRO\Desktop\RT-QuIC Data\Gage's RT-QuIC Data\2025\20250714_r2_GR_USDA-LNs_RT-QuIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowde002\Documents\Projects\usda-validation\raw\necropsy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6914381B-3718-48B8-8EB0-A3E89A4D2847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6C26DD-7F39-4F81-BB4F-93FC64F60EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{00785452-4EFE-4514-8C0A-2937BDF42666}"/>
+    <workbookView xWindow="-28905" yWindow="105" windowWidth="14610" windowHeight="15585" xr2:uid="{00785452-4EFE-4514-8C0A-2937BDF42666}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -32,12 +32,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="159">
   <si>
     <t>User: USER</t>
   </si>
@@ -1135,13 +1138,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF225DC8-1ED8-46BD-BF51-C70A4272B672}">
   <dimension ref="A3:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1610,38 +1619,38 @@
       <c r="B27" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>145</v>
+      <c r="C27" s="12">
+        <v>2276</v>
+      </c>
+      <c r="D27" s="12">
+        <v>2277</v>
+      </c>
+      <c r="E27" s="12">
+        <v>2278</v>
+      </c>
+      <c r="F27" s="12">
+        <v>2279</v>
+      </c>
+      <c r="G27" s="12">
+        <v>2280</v>
+      </c>
+      <c r="H27" s="12">
+        <v>2281</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1983</v>
+      </c>
+      <c r="J27" s="12">
+        <v>2282</v>
+      </c>
+      <c r="K27" s="12">
+        <v>2283</v>
+      </c>
+      <c r="L27" s="12">
+        <v>2284</v>
+      </c>
+      <c r="M27" s="13">
+        <v>1984</v>
       </c>
       <c r="O27" s="21"/>
     </row>
@@ -1652,38 +1661,38 @@
       <c r="B28" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M28" s="15" t="s">
-        <v>145</v>
+      <c r="C28" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D28" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E28" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F28" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G28" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H28" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I28" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J28" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K28" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L28" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M28" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1693,38 +1702,38 @@
       <c r="B29" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M29" s="15" t="s">
-        <v>145</v>
+      <c r="C29" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D29" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E29" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F29" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G29" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H29" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I29" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J29" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K29" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L29" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M29" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1734,38 +1743,38 @@
       <c r="B30" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L30" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M30" s="15" t="s">
-        <v>145</v>
+      <c r="C30" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D30" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E30" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F30" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G30" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H30" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I30" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J30" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K30" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L30" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M30" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1775,38 +1784,38 @@
       <c r="B31" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L31" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M31" s="15" t="s">
-        <v>145</v>
+      <c r="C31" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E31" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F31" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G31" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H31" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I31" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J31" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K31" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L31" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M31" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1816,38 +1825,38 @@
       <c r="B32" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L32" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M32" s="15" t="s">
-        <v>145</v>
+      <c r="C32" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D32" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E32" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F32" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G32" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H32" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I32" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J32" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K32" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L32" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M32" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -1857,38 +1866,38 @@
       <c r="B33" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="L33" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M33" s="15" t="s">
-        <v>145</v>
+      <c r="C33" s="14">
+        <v>2276</v>
+      </c>
+      <c r="D33" s="14">
+        <v>2277</v>
+      </c>
+      <c r="E33" s="14">
+        <v>2278</v>
+      </c>
+      <c r="F33" s="14">
+        <v>2279</v>
+      </c>
+      <c r="G33" s="14">
+        <v>2280</v>
+      </c>
+      <c r="H33" s="14">
+        <v>2281</v>
+      </c>
+      <c r="I33" s="14">
+        <v>1983</v>
+      </c>
+      <c r="J33" s="14">
+        <v>2282</v>
+      </c>
+      <c r="K33" s="14">
+        <v>2283</v>
+      </c>
+      <c r="L33" s="14">
+        <v>2284</v>
+      </c>
+      <c r="M33" s="15">
+        <v>1984</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -1898,38 +1907,38 @@
       <c r="B34" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="M34" s="18" t="s">
-        <v>145</v>
+      <c r="C34" s="17">
+        <v>2276</v>
+      </c>
+      <c r="D34" s="17">
+        <v>2277</v>
+      </c>
+      <c r="E34" s="17">
+        <v>2278</v>
+      </c>
+      <c r="F34" s="17">
+        <v>2279</v>
+      </c>
+      <c r="G34" s="17">
+        <v>2280</v>
+      </c>
+      <c r="H34" s="17">
+        <v>2281</v>
+      </c>
+      <c r="I34" s="17">
+        <v>1983</v>
+      </c>
+      <c r="J34" s="17">
+        <v>2282</v>
+      </c>
+      <c r="K34" s="17">
+        <v>2283</v>
+      </c>
+      <c r="L34" s="17">
+        <v>2284</v>
+      </c>
+      <c r="M34" s="18">
+        <v>1984</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>